<commit_message>
Escaleta corregida y mapa simplificado CN_09_04_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion04/ESCALETA CN_09_04_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion04/ESCALETA CN_09_04_CO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="259">
   <si>
     <t>Asignatura</t>
   </si>
@@ -397,9 +397,6 @@
   </si>
   <si>
     <t>Modelos de clasificación biológica</t>
-  </si>
-  <si>
-    <t>Interctivo que expone los modelos tradicional y moderno de clasificación biológica</t>
   </si>
   <si>
     <t>La primera ficha explia qué es la clasificación biológica y por qué es importante. Segunda ficha explica el modelo tradicional de clasificación, con procariotas y eucariotas, y 5 reinos incluyendo el mónera. La tercera ficha explica los 3 dominios, con un reino cada uno de los dos primeros y con 4 reinos el eucariota. Se debe explicar que Archaea es en latín y arquea en español, lo mismo para Eukarya y Fungi.</t>
@@ -475,15 +472,9 @@
     <t>Fundamentos de la taxonomía</t>
   </si>
   <si>
-    <t>Actiidad que repasa aspectos básicos de la taxonomía</t>
-  </si>
-  <si>
     <t xml:space="preserve">Se debe hacer un texto con los términos taxa, taxón, análogos, homólogos y binomial. Expandir si se quiere. </t>
   </si>
   <si>
-    <t>Interactivo que explica las categorías taxonómicas</t>
-  </si>
-  <si>
     <t>Se hace una imagen que englobe las distintas categorías taxonómicas; puede ser en forma de circulos, uno dentro de otro, por ejemplo. Los círculos hablan de dominio, reino, filo/división, clase, orden, familia, género y especie. Con el botón de información se explica que esta es una estructura jerarquica, y lo que haga falta para entender el recurso. En cada categoría, se pone como ejemplo la clasificación del ser humano (por ejemplo, familia hominidae, phylum chordata, etc.). En la aprte de especie se debe hacer énfasis en la importancia de esta categoría, y explicar que es dificil definirla, pues la definición más común sólo aplica para organismos con reproducción sexual. Decir que se está trabajando aún en eso.</t>
   </si>
   <si>
@@ -649,24 +640,6 @@
     <t xml:space="preserve">Competencias: juega a reconocer las características de los dominios y los reinos de la naturaleza </t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad que propone realizar un juego en el que a partir de pistas, se reconocen organismos de diferentes dominios y reinos. </t>
-  </si>
-  <si>
-    <t>Dominios y reinos de la naturaleza</t>
-  </si>
-  <si>
-    <t>Preguntar por importancia de la clasificación, modelos tradicional y moderno, y cosas de taxonomía (taxa, taxón, caracteristica homóloga, especie, categorías…)</t>
-  </si>
-  <si>
-    <t>Preguntar por característoicas de organismos de los 3 dominios y los 6 reinos</t>
-  </si>
-  <si>
-    <t>Actividad que sirve para evaluar la comprensión de la clasificación biológica</t>
-  </si>
-  <si>
-    <t>Actividad que sirve para evaluar la comprensión de los dominios y reinos de la naturaleza</t>
-  </si>
-  <si>
     <t>Fin de unidad</t>
   </si>
   <si>
@@ -748,9 +721,6 @@
     <t>Recurso M101A-04</t>
   </si>
   <si>
-    <t>Recurso M101A-05</t>
-  </si>
-  <si>
     <t>Recurso M10A-01</t>
   </si>
   <si>
@@ -778,25 +748,58 @@
     <t>Recurso M4A-02</t>
   </si>
   <si>
-    <t>Recurso M4A-03</t>
-  </si>
-  <si>
     <t>Recurso M1B-01</t>
   </si>
   <si>
-    <t>Recurso M102B-01</t>
-  </si>
-  <si>
-    <t>Recurso M102B-02</t>
-  </si>
-  <si>
-    <t>Recurso M102B-03</t>
-  </si>
-  <si>
     <t>Recurso M4A-04</t>
   </si>
   <si>
     <t>Recurso M101AP-02</t>
+  </si>
+  <si>
+    <t>Recurso M102AB-03</t>
+  </si>
+  <si>
+    <t>Recurso M102AB-02</t>
+  </si>
+  <si>
+    <t>Recurso M102AB-01</t>
+  </si>
+  <si>
+    <t>Se pide organizar las categorías taxonómicas de la más general (dominio) a la menos general (género).</t>
+  </si>
+  <si>
+    <t>El orden de los taxones</t>
+  </si>
+  <si>
+    <t>Actividad acerca de la jerarquía de los taxones</t>
+  </si>
+  <si>
+    <t>Actividad en la que se debe indicar a qué categorías taxonómicas pertenecen algunos organismos</t>
+  </si>
+  <si>
+    <t>¿A qué taxones perteneces estos organismos?</t>
+  </si>
+  <si>
+    <t>Interactivo que expone los modelos tradicional y moderno de clasificación biológica</t>
+  </si>
+  <si>
+    <t>Actividad que repasa aspectos básicos de la taxonomía</t>
+  </si>
+  <si>
+    <t>Interactivo que explica las categorías taxonómicas principales</t>
+  </si>
+  <si>
+    <t>Las palabras de la sopa de letras son dominio, reino, filo, división, clase, orden, familia, género y especie</t>
+  </si>
+  <si>
+    <t>Actividad que propone realizar un juego en el que a partir de pistas se reconocen organismos de diferentes dominios y reinos</t>
+  </si>
+  <si>
+    <t>Mapa conceptual del tema La clasificación biológica</t>
+  </si>
+  <si>
+    <t>Evaluación</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1026,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1087,6 +1090,16 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1132,14 +1145,10 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3407,7 +3416,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U121"/>
+  <dimension ref="A1:U113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:A2"/>
@@ -3429,7 +3438,7 @@
     <col min="13" max="13" width="13.85546875" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" customWidth="1"/>
     <col min="15" max="15" width="29.28515625" style="15" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="15" customWidth="1"/>
+    <col min="16" max="16" width="21.5703125" style="56" customWidth="1"/>
     <col min="17" max="17" width="16.140625" style="15" customWidth="1"/>
     <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -3438,94 +3447,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="38" t="s">
+      <c r="N1" s="49"/>
+      <c r="O1" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="47" t="s">
+      <c r="P1" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="R1" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="S1" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="49" t="s">
+      <c r="T1" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="U1" s="52" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="41"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="45"/>
       <c r="M2" s="13" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="48"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="52"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -3537,14 +3546,14 @@
       <c r="C3" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="39" t="s">
         <v>125</v>
       </c>
       <c r="F3" s="19"/>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="36" t="s">
         <v>126</v>
       </c>
       <c r="H3" s="35">
@@ -3554,7 +3563,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>127</v>
+        <v>252</v>
       </c>
       <c r="K3" s="22" t="s">
         <v>20</v>
@@ -3567,25 +3576,25 @@
       </c>
       <c r="N3" s="23"/>
       <c r="O3" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="P3" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="P3" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q3" s="25">
         <v>6</v>
       </c>
       <c r="R3" s="26" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="S3" s="25" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="T3" s="27" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U3" s="25" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3598,15 +3607,15 @@
       <c r="C4" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="37" t="s">
         <v>124</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H4" s="28">
         <v>2</v>
@@ -3615,7 +3624,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K4" s="22" t="s">
         <v>20</v>
@@ -3628,25 +3637,25 @@
         <v>43</v>
       </c>
       <c r="O4" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="P4" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="P4" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q4" s="31">
         <v>6</v>
       </c>
       <c r="R4" s="32" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S4" s="31" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T4" s="33" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="U4" s="31" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3659,15 +3668,15 @@
       <c r="C5" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="37" t="s">
         <v>124</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H5" s="28">
         <v>3</v>
@@ -3676,7 +3685,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K5" s="22" t="s">
         <v>20</v>
@@ -3689,25 +3698,25 @@
       </c>
       <c r="N5" s="23"/>
       <c r="O5" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="P5" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="P5" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q5" s="31">
         <v>6</v>
       </c>
       <c r="R5" s="32" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="S5" s="31" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="T5" s="33" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="U5" s="31" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3720,15 +3729,15 @@
       <c r="C6" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="37" t="s">
         <v>124</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H6" s="28">
         <v>4</v>
@@ -3737,7 +3746,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K6" s="22" t="s">
         <v>20</v>
@@ -3750,25 +3759,25 @@
         <v>52</v>
       </c>
       <c r="O6" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="P6" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="P6" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q6" s="31">
         <v>6</v>
       </c>
       <c r="R6" s="32" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S6" s="31" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T6" s="33" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="U6" s="31" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3781,15 +3790,15 @@
       <c r="C7" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="53" t="s">
-        <v>140</v>
+      <c r="D7" s="38" t="s">
+        <v>139</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H7" s="35">
         <v>5</v>
@@ -3798,7 +3807,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K7" s="22" t="s">
         <v>20</v>
@@ -3811,25 +3820,25 @@
       </c>
       <c r="N7" s="23"/>
       <c r="O7" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="P7" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="P7" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q7" s="31">
         <v>6</v>
       </c>
       <c r="R7" s="32" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="S7" s="31" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="T7" s="33" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="U7" s="31" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3843,14 +3852,14 @@
         <v>123</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H8" s="28">
         <v>6</v>
@@ -3859,7 +3868,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>150</v>
+        <v>253</v>
       </c>
       <c r="K8" s="22" t="s">
         <v>20</v>
@@ -3872,25 +3881,25 @@
         <v>28</v>
       </c>
       <c r="O8" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="P8" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="P8" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q8" s="31">
         <v>6</v>
       </c>
       <c r="R8" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="S8" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="T8" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="S8" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="T8" s="33" t="s">
-        <v>244</v>
-      </c>
       <c r="U8" s="31" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3904,14 +3913,14 @@
         <v>123</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="29" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H9" s="28">
         <v>7</v>
@@ -3920,7 +3929,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>152</v>
+        <v>254</v>
       </c>
       <c r="K9" s="22" t="s">
         <v>20</v>
@@ -3933,25 +3942,25 @@
       </c>
       <c r="N9" s="23"/>
       <c r="O9" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="P9" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="P9" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q9" s="31">
         <v>6</v>
       </c>
       <c r="R9" s="32" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="S9" s="31" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="T9" s="33" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="U9" s="31" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3965,54 +3974,54 @@
         <v>123</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>148</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="F10" s="28"/>
       <c r="G10" s="29" t="s">
-        <v>147</v>
+        <v>248</v>
       </c>
       <c r="H10" s="28">
         <v>8</v>
       </c>
       <c r="I10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="P10" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="P10" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="R10" s="32" t="s">
-        <v>219</v>
-      </c>
-      <c r="S10" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="T10" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="U10" s="31" t="s">
-        <v>222</v>
+      <c r="Q10" s="6">
+        <v>6</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="U10" s="6" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4026,56 +4035,54 @@
         <v>123</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="F11" s="28" t="s">
-        <v>148</v>
-      </c>
       <c r="G11" s="29" t="s">
-        <v>156</v>
+        <v>212</v>
       </c>
       <c r="H11" s="28">
         <v>9</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M11" s="23"/>
-      <c r="N11" s="23" t="s">
-        <v>51</v>
-      </c>
+      <c r="N11" s="23"/>
       <c r="O11" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="P11" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="P11" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="6">
-        <v>6</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="S11" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="T11" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="U11" s="6" t="s">
-        <v>237</v>
+      <c r="Q11" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="R11" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="S11" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="T11" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="U11" s="31" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4089,14 +4096,16 @@
         <v>123</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F12" s="28"/>
+        <v>146</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>147</v>
+      </c>
       <c r="G12" s="29" t="s">
-        <v>144</v>
+        <v>251</v>
       </c>
       <c r="H12" s="28">
         <v>10</v>
@@ -4105,7 +4114,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>145</v>
+        <v>250</v>
       </c>
       <c r="K12" s="22" t="s">
         <v>20</v>
@@ -4115,28 +4124,28 @@
       </c>
       <c r="M12" s="23"/>
       <c r="N12" s="23" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="O12" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="P12" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="P12" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q12" s="6">
         <v>6</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S12" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="T12" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="T12" s="7" t="s">
-        <v>238</v>
-      </c>
       <c r="U12" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4150,52 +4159,56 @@
         <v>123</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="3" t="s">
-        <v>161</v>
+        <v>139</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>153</v>
       </c>
       <c r="H13" s="28">
         <v>11</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>162</v>
+        <v>20</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>154</v>
       </c>
       <c r="K13" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="N13" s="12"/>
-      <c r="O13" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="P13" s="24" t="s">
-        <v>19</v>
+      <c r="L13" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="P13" s="55" t="s">
+        <v>20</v>
       </c>
       <c r="Q13" s="6">
         <v>6</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="T13" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="U13" s="6" t="s">
         <v>228</v>
-      </c>
-      <c r="U13" s="6" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4209,14 +4222,14 @@
         <v>123</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="3" t="s">
-        <v>170</v>
+        <v>135</v>
+      </c>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="H14" s="28">
         <v>12</v>
@@ -4224,39 +4237,39 @@
       <c r="I14" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>167</v>
+      <c r="J14" s="30" t="s">
+        <v>144</v>
       </c>
       <c r="K14" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="L14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="P14" s="24" t="s">
+      <c r="M14" s="23"/>
+      <c r="N14" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O14" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="P14" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q14" s="6">
         <v>6</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4270,54 +4283,52 @@
         <v>123</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>165</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="14"/>
       <c r="G15" s="3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="H15" s="28">
         <v>13</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="K15" s="22" t="s">
         <v>20</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N15" s="12"/>
       <c r="O15" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="P15" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="P15" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q15" s="6">
         <v>6</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4331,14 +4342,14 @@
         <v>123</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H16" s="28">
         <v>14</v>
@@ -4347,7 +4358,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K16" s="22" t="s">
         <v>20</v>
@@ -4360,25 +4371,25 @@
         <v>27</v>
       </c>
       <c r="O16" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="P16" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="P16" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q16" s="6">
         <v>6</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="U16" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4392,14 +4403,14 @@
         <v>123</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="H17" s="28">
         <v>15</v>
@@ -4408,7 +4419,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="K17" s="22" t="s">
         <v>20</v>
@@ -4418,28 +4429,28 @@
       </c>
       <c r="M17" s="12"/>
       <c r="N17" s="12" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="P17" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="P17" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q17" s="6">
         <v>6</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T17" s="7" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="U17" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4453,14 +4464,14 @@
         <v>123</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="H18" s="28">
         <v>16</v>
@@ -4469,7 +4480,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="K18" s="22" t="s">
         <v>20</v>
@@ -4479,28 +4490,28 @@
       </c>
       <c r="M18" s="12"/>
       <c r="N18" s="12" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="P18" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="P18" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q18" s="6">
         <v>6</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4514,58 +4525,60 @@
         <v>123</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H19" s="35">
+        <v>169</v>
+      </c>
+      <c r="H19" s="28">
         <v>17</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="K19" s="22" t="s">
         <v>20</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N19" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="O19" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="P19" s="24" t="s">
-        <v>19</v>
+        <v>174</v>
+      </c>
+      <c r="P19" s="55" t="s">
+        <v>20</v>
       </c>
       <c r="Q19" s="6">
         <v>6</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="U19" s="6" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="B20" s="9" t="s">
         <v>122</v>
       </c>
@@ -4573,14 +4586,14 @@
         <v>123</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>181</v>
+        <v>135</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="3" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="H20" s="28">
         <v>18</v>
@@ -4589,7 +4602,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="K20" s="22" t="s">
         <v>20</v>
@@ -4599,28 +4612,28 @@
       </c>
       <c r="M20" s="12"/>
       <c r="N20" s="12" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="P20" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="P20" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q20" s="6">
         <v>6</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S20" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4634,23 +4647,23 @@
         <v>123</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="H21" s="28">
+        <v>180</v>
+      </c>
+      <c r="H21" s="35">
         <v>19</v>
       </c>
       <c r="I21" s="19" t="s">
         <v>19</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="K21" s="22" t="s">
         <v>20</v>
@@ -4663,31 +4676,29 @@
       </c>
       <c r="N21" s="12"/>
       <c r="O21" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="P21" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="P21" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q21" s="6">
         <v>6</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="S21" s="6" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="U21" s="6" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="A22" s="8"/>
       <c r="B22" s="9" t="s">
         <v>122</v>
       </c>
@@ -4695,14 +4706,14 @@
         <v>123</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H22" s="28">
         <v>20</v>
@@ -4724,25 +4735,25 @@
         <v>32</v>
       </c>
       <c r="O22" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="P22" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="P22" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q22" s="6">
         <v>6</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S22" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="U22" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4756,23 +4767,23 @@
         <v>123</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="H23" s="35">
+        <v>190</v>
+      </c>
+      <c r="H23" s="28">
         <v>21</v>
       </c>
       <c r="I23" s="19" t="s">
         <v>19</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="K23" s="22" t="s">
         <v>20</v>
@@ -4781,29 +4792,29 @@
         <v>5</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="N23" s="12"/>
       <c r="O23" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="P23" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="P23" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q23" s="6">
         <v>6</v>
       </c>
       <c r="R23" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="T23" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="S23" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="T23" s="7" t="s">
-        <v>233</v>
-      </c>
       <c r="U23" s="6" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4817,14 +4828,14 @@
         <v>123</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H24" s="28">
         <v>22</v>
@@ -4833,7 +4844,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K24" s="22" t="s">
         <v>20</v>
@@ -4843,28 +4854,28 @@
       </c>
       <c r="M24" s="12"/>
       <c r="N24" s="12" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="O24" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="P24" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="P24" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q24" s="6">
         <v>6</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T24" s="7" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="U24" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4878,54 +4889,54 @@
         <v>123</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H25" s="28">
+        <v>179</v>
+      </c>
+      <c r="H25" s="35">
         <v>23</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="K25" s="22" t="s">
         <v>20</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12" t="s">
-        <v>52</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="N25" s="12"/>
       <c r="O25" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="P25" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="P25" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q25" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="S25" s="6" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="T25" s="7" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="U25" s="6" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4939,12 +4950,14 @@
         <v>123</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E26" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>179</v>
+      </c>
       <c r="F26" s="14"/>
       <c r="G26" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H26" s="28">
         <v>24</v>
@@ -4953,7 +4966,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="K26" s="22" t="s">
         <v>20</v>
@@ -4963,28 +4976,28 @@
       </c>
       <c r="M26" s="12"/>
       <c r="N26" s="12" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="P26" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="P26" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q26" s="6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="R26" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S26" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T26" s="7" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="U26" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4998,21 +5011,23 @@
         <v>123</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E27" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="F27" s="14"/>
       <c r="G27" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="H27" s="35">
+        <v>185</v>
+      </c>
+      <c r="H27" s="28">
         <v>25</v>
       </c>
       <c r="I27" s="19" t="s">
         <v>20</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="K27" s="22" t="s">
         <v>20</v>
@@ -5022,28 +5037,28 @@
       </c>
       <c r="M27" s="12"/>
       <c r="N27" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O27" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="P27" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="P27" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q27" s="6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="R27" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S27" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="U27" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5057,12 +5072,12 @@
         <v>123</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="14"/>
       <c r="G28" s="3" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="H28" s="28">
         <v>26</v>
@@ -5071,7 +5086,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="K28" s="22" t="s">
         <v>20</v>
@@ -5084,25 +5099,25 @@
         <v>54</v>
       </c>
       <c r="O28" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="P28" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="P28" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q28" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S28" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T28" s="7" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="U28" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5116,21 +5131,21 @@
         <v>123</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="14"/>
       <c r="G29" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="H29" s="28">
+        <v>202</v>
+      </c>
+      <c r="H29" s="35">
         <v>27</v>
       </c>
       <c r="I29" s="19" t="s">
         <v>20</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="K29" s="22" t="s">
         <v>20</v>
@@ -5140,28 +5155,28 @@
       </c>
       <c r="M29" s="12"/>
       <c r="N29" s="12" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="O29" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="P29" s="24" t="s">
-        <v>20</v>
+        <v>138</v>
+      </c>
+      <c r="P29" s="55" t="s">
+        <v>19</v>
       </c>
       <c r="Q29" s="6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S29" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T29" s="7" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="U29" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5175,12 +5190,12 @@
         <v>123</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="14"/>
       <c r="G30" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H30" s="28">
         <v>28</v>
@@ -5189,7 +5204,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="K30" s="22" t="s">
         <v>20</v>
@@ -5199,28 +5214,28 @@
       </c>
       <c r="M30" s="12"/>
       <c r="N30" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="O30" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="P30" s="24" t="s">
-        <v>20</v>
+        <v>138</v>
+      </c>
+      <c r="P30" s="55" t="s">
+        <v>19</v>
       </c>
       <c r="Q30" s="6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="R30" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S30" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T30" s="7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="U30" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5234,7 +5249,7 @@
         <v>123</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="14"/>
@@ -5248,7 +5263,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>123</v>
+        <v>257</v>
       </c>
       <c r="K31" s="22" t="s">
         <v>20</v>
@@ -5259,7 +5274,7 @@
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="24" t="s">
+      <c r="P31" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q31" s="6"/>
@@ -5279,12 +5294,12 @@
         <v>123</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="14"/>
       <c r="G32" s="3" t="s">
-        <v>123</v>
+        <v>258</v>
       </c>
       <c r="H32" s="28">
         <v>30</v>
@@ -5293,7 +5308,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="K32" s="22" t="s">
         <v>20</v>
@@ -5306,23 +5321,23 @@
         <v>32</v>
       </c>
       <c r="O32" s="14"/>
-      <c r="P32" s="24" t="s">
+      <c r="P32" s="55" t="s">
         <v>19</v>
       </c>
       <c r="Q32" s="6">
         <v>6</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S32" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="U32" s="6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5336,12 +5351,12 @@
         <v>123</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="14"/>
       <c r="G33" s="3" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="H33" s="28">
         <v>31</v>
@@ -5350,7 +5365,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="K33" s="22" t="s">
         <v>20</v>
@@ -5363,503 +5378,207 @@
         <v>53</v>
       </c>
       <c r="O33" s="14"/>
-      <c r="P33" s="24" t="s">
-        <v>19</v>
+      <c r="P33" s="55" t="s">
+        <v>20</v>
       </c>
       <c r="Q33" s="6">
         <v>6</v>
       </c>
       <c r="R33" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="S33" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="U33" s="6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="28">
-        <v>32</v>
-      </c>
-      <c r="I34" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L34" s="11"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="6"/>
-      <c r="T34" s="7"/>
-      <c r="U34" s="6"/>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="35">
-        <v>33</v>
-      </c>
-      <c r="I35" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L35" s="11"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="6"/>
-      <c r="T35" s="7"/>
-      <c r="U35" s="6"/>
-    </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="28">
-        <v>34</v>
-      </c>
-      <c r="I36" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J36" s="4"/>
-      <c r="K36" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" s="11"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="7"/>
-      <c r="U36" s="6"/>
-    </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="28">
-        <v>35</v>
-      </c>
-      <c r="I37" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J37" s="4"/>
-      <c r="K37" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L37" s="11"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="7"/>
-      <c r="U37" s="6"/>
-    </row>
-    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="28">
-        <v>36</v>
-      </c>
-      <c r="I38" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="11"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="7"/>
-      <c r="U38" s="6"/>
-    </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="35">
-        <v>37</v>
-      </c>
-      <c r="I39" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J39" s="4"/>
-      <c r="K39" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L39" s="11"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="6"/>
-      <c r="T39" s="7"/>
-      <c r="U39" s="6"/>
-    </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="28">
-        <v>38</v>
-      </c>
-      <c r="I40" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J40" s="4"/>
-      <c r="K40" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" s="11"/>
-      <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="6"/>
-      <c r="T40" s="7"/>
-      <c r="U40" s="6"/>
-    </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="28">
-        <v>39</v>
-      </c>
-      <c r="I41" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J41" s="4"/>
-      <c r="K41" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L41" s="11"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="6"/>
-      <c r="T41" s="7"/>
-      <c r="U41" s="6"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
         <v>117</v>
       </c>
     </row>
@@ -5887,8 +5606,8 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P41 I3:I41">
-      <formula1>$D$48:$D$49</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I33 P3:P33">
+      <formula1>$D$40:$D$41</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5900,31 +5619,31 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N41</xm:sqref>
+          <xm:sqref>N3:N33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A41</xm:sqref>
+          <xm:sqref>A3:A33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K41</xm:sqref>
+          <xm:sqref>K3:K33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L41</xm:sqref>
+          <xm:sqref>L3:L33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M41</xm:sqref>
+          <xm:sqref>M3:M33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Corrección tipología de un recurso
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion04/ESCALETA CN_09_04_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion04/ESCALETA CN_09_04_CO.xlsx
@@ -423,16 +423,6 @@
     <t>Consolidación</t>
   </si>
   <si>
-    <t xml:space="preserve">Mediante este recurso se presenta un panorama histórico de la clasificación biológica, haciendo énfasis en sus representantes y las contribuciones de cada uno de ellos. Los botones de la izquierda hablan sobre: • Aristóteles (384 a.C.)
-• Carlos Linneo (1707 – 1778)
-• Erns Haeckel (1834 – 1919)
-• Herbert Copeland (1902 – 1968)
-• Robert Whittaker (1920 – 1980)
-• Lynn Margulis (1938 – 2011)
-• Carl Woese (1928 – 2012)
-</t>
-  </si>
-  <si>
     <t>La taxonomía</t>
   </si>
   <si>
@@ -801,6 +791,9 @@
   </si>
   <si>
     <t>Recurso M10A-03</t>
+  </si>
+  <si>
+    <t>Mediante este recurso se presenta un panorama histórico de la clasificación biológica, haciendo énfasis en sus representantes y las contribuciones de cada uno de ellos. Los botones de la izquierda hablan sobre: • Aristóteles (384 a.C.) • Carlos Linneo (1707 – 1778) • Erns Haeckel (1834 – 1919) • Herbert Copeland (1902 – 1968) • Robert Whittaker (1920 – 1980) • Lynn Margulis (1938 – 2011) • Carl Woese (1928 – 2012)</t>
   </si>
 </sst>
 </file>
@@ -1110,25 +1103,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1153,6 +1134,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3422,8 +3415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3451,94 +3444,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="44" t="s">
+      <c r="N1" s="52"/>
+      <c r="O1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="43" t="s">
+      <c r="P1" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="45" t="s">
+      <c r="Q1" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="S1" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="U1" s="55" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="52"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="48"/>
       <c r="M2" s="13" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="55"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -3551,7 +3544,7 @@
         <v>123</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E3" s="38" t="s">
         <v>124</v>
@@ -3567,7 +3560,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K3" s="21" t="s">
         <v>20</v>
@@ -3589,16 +3582,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="S3" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="S3" s="24" t="s">
+      <c r="T3" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="T3" s="26" t="s">
+      <c r="U3" s="24" t="s">
         <v>201</v>
-      </c>
-      <c r="U3" s="24" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3612,7 +3605,7 @@
         <v>123</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>128</v>
@@ -3650,16 +3643,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="S4" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="S4" s="30" t="s">
-        <v>209</v>
-      </c>
       <c r="T4" s="32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U4" s="30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3673,7 +3666,7 @@
         <v>123</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>127</v>
@@ -3695,14 +3688,14 @@
         <v>20</v>
       </c>
       <c r="L5" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M5" s="22" t="s">
         <v>62</v>
       </c>
       <c r="N5" s="22"/>
       <c r="O5" s="33" t="s">
-        <v>135</v>
+        <v>258</v>
       </c>
       <c r="P5" s="39" t="s">
         <v>19</v>
@@ -3711,16 +3704,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="S5" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="S5" s="30" t="s">
-        <v>200</v>
-      </c>
       <c r="T5" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U5" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3734,14 +3727,14 @@
         <v>123</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H6" s="27">
         <v>4</v>
@@ -3750,7 +3743,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>20</v>
@@ -3763,7 +3756,7 @@
         <v>52</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P6" s="39" t="s">
         <v>19</v>
@@ -3772,16 +3765,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="S6" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="S6" s="30" t="s">
+      <c r="T6" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="T6" s="32" t="s">
+      <c r="U6" s="30" t="s">
         <v>210</v>
-      </c>
-      <c r="U6" s="30" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3795,14 +3788,14 @@
         <v>123</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H7" s="34">
         <v>5</v>
@@ -3811,7 +3804,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K7" s="21" t="s">
         <v>20</v>
@@ -3824,7 +3817,7 @@
       </c>
       <c r="N7" s="22"/>
       <c r="O7" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P7" s="39" t="s">
         <v>19</v>
@@ -3833,16 +3826,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="S7" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="S7" s="30" t="s">
-        <v>200</v>
-      </c>
       <c r="T7" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U7" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3856,14 +3849,14 @@
         <v>123</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H8" s="27">
         <v>6</v>
@@ -3872,7 +3865,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>20</v>
@@ -3885,7 +3878,7 @@
         <v>28</v>
       </c>
       <c r="O8" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P8" s="39" t="s">
         <v>19</v>
@@ -3894,16 +3887,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="S8" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="S8" s="30" t="s">
-        <v>209</v>
-      </c>
       <c r="T8" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="U8" s="30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3917,14 +3910,14 @@
         <v>123</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H9" s="27">
         <v>7</v>
@@ -3933,7 +3926,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>20</v>
@@ -3946,7 +3939,7 @@
       </c>
       <c r="N9" s="22"/>
       <c r="O9" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P9" s="39" t="s">
         <v>19</v>
@@ -3955,16 +3948,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="S9" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="S9" s="30" t="s">
-        <v>200</v>
-      </c>
       <c r="T9" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="U9" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3978,14 +3971,14 @@
         <v>123</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H10" s="27">
         <v>8</v>
@@ -3994,7 +3987,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>20</v>
@@ -4007,7 +4000,7 @@
         <v>45</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P10" s="39" t="s">
         <v>19</v>
@@ -4016,16 +4009,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S10" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S10" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T10" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="U10" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4039,16 +4032,16 @@
         <v>123</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="F11" s="27" t="s">
-        <v>143</v>
-      </c>
       <c r="G11" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H11" s="27">
         <v>9</v>
@@ -4057,7 +4050,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>19</v>
@@ -4068,25 +4061,25 @@
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
       <c r="O11" s="27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P11" s="39" t="s">
         <v>19</v>
       </c>
       <c r="Q11" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="R11" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="R11" s="31" t="s">
+      <c r="S11" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="S11" s="30" t="s">
+      <c r="T11" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="T11" s="32" t="s">
+      <c r="U11" s="30" t="s">
         <v>197</v>
-      </c>
-      <c r="U11" s="30" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4100,16 +4093,16 @@
         <v>123</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>143</v>
-      </c>
       <c r="G12" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H12" s="27">
         <v>10</v>
@@ -4118,7 +4111,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K12" s="21" t="s">
         <v>20</v>
@@ -4131,7 +4124,7 @@
         <v>43</v>
       </c>
       <c r="O12" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P12" s="39" t="s">
         <v>19</v>
@@ -4140,16 +4133,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S12" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S12" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T12" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="U12" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4163,16 +4156,16 @@
         <v>123</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="F13" s="27" t="s">
-        <v>143</v>
-      </c>
       <c r="G13" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H13" s="27">
         <v>11</v>
@@ -4181,7 +4174,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>20</v>
@@ -4194,7 +4187,7 @@
         <v>51</v>
       </c>
       <c r="O13" s="27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P13" s="39" t="s">
         <v>20</v>
@@ -4203,16 +4196,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S13" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S13" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T13" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="U13" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4226,14 +4219,14 @@
         <v>123</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H14" s="27">
         <v>12</v>
@@ -4242,7 +4235,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K14" s="21" t="s">
         <v>20</v>
@@ -4255,7 +4248,7 @@
         <v>52</v>
       </c>
       <c r="O14" s="42" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P14" s="39" t="s">
         <v>19</v>
@@ -4264,16 +4257,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S14" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S14" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T14" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4287,12 +4280,12 @@
         <v>123</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="14"/>
       <c r="G15" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H15" s="27">
         <v>13</v>
@@ -4301,7 +4294,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>20</v>
@@ -4314,7 +4307,7 @@
       </c>
       <c r="N15" s="12"/>
       <c r="O15" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P15" s="39" t="s">
         <v>19</v>
@@ -4323,16 +4316,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="S15" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="S15" s="6" t="s">
-        <v>200</v>
-      </c>
       <c r="T15" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4346,14 +4339,14 @@
         <v>123</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H16" s="27">
         <v>14</v>
@@ -4362,7 +4355,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K16" s="21" t="s">
         <v>20</v>
@@ -4375,7 +4368,7 @@
         <v>27</v>
       </c>
       <c r="O16" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P16" s="39" t="s">
         <v>19</v>
@@ -4384,16 +4377,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S16" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S16" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T16" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U16" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4407,14 +4400,14 @@
         <v>123</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
@@ -4423,7 +4416,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K17" s="21" t="s">
         <v>20</v>
@@ -4436,7 +4429,7 @@
         <v>27</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P17" s="39" t="s">
         <v>19</v>
@@ -4445,16 +4438,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S17" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S17" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T17" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U17" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4468,14 +4461,14 @@
         <v>123</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
@@ -4484,7 +4477,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K18" s="21" t="s">
         <v>20</v>
@@ -4497,7 +4490,7 @@
         <v>27</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P18" s="39" t="s">
         <v>19</v>
@@ -4506,16 +4499,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S18" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S18" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T18" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4529,14 +4522,14 @@
         <v>123</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H19" s="27">
         <v>17</v>
@@ -4545,7 +4538,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>20</v>
@@ -4558,7 +4551,7 @@
         <v>43</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P19" s="39" t="s">
         <v>20</v>
@@ -4567,16 +4560,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S19" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S19" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T19" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U19" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4590,14 +4583,14 @@
         <v>123</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H20" s="27">
         <v>18</v>
@@ -4606,7 +4599,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>20</v>
@@ -4619,7 +4612,7 @@
         <v>52</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P20" s="39" t="s">
         <v>19</v>
@@ -4628,16 +4621,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S20" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S20" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T20" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4651,12 +4644,12 @@
         <v>123</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="14"/>
       <c r="G21" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H21" s="34">
         <v>19</v>
@@ -4665,7 +4658,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K21" s="21" t="s">
         <v>20</v>
@@ -4678,7 +4671,7 @@
       </c>
       <c r="N21" s="12"/>
       <c r="O21" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P21" s="39" t="s">
         <v>19</v>
@@ -4687,16 +4680,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="S21" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="S21" s="6" t="s">
-        <v>200</v>
-      </c>
       <c r="T21" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="U21" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4710,14 +4703,14 @@
         <v>123</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H22" s="27">
         <v>20</v>
@@ -4726,7 +4719,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>20</v>
@@ -4739,7 +4732,7 @@
         <v>32</v>
       </c>
       <c r="O22" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P22" s="39" t="s">
         <v>19</v>
@@ -4748,16 +4741,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S22" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S22" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T22" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U22" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4771,14 +4764,14 @@
         <v>123</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H23" s="27">
         <v>21</v>
@@ -4787,7 +4780,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>20</v>
@@ -4800,7 +4793,7 @@
         <v>32</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P23" s="39" t="s">
         <v>19</v>
@@ -4809,16 +4802,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S23" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S23" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T23" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="U23" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4832,14 +4825,14 @@
         <v>123</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H24" s="27">
         <v>22</v>
@@ -4848,7 +4841,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>20</v>
@@ -4861,7 +4854,7 @@
         <v>23</v>
       </c>
       <c r="O24" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P24" s="39" t="s">
         <v>19</v>
@@ -4870,16 +4863,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S24" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S24" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T24" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U24" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4893,14 +4886,14 @@
         <v>123</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H25" s="27">
         <v>23</v>
@@ -4909,7 +4902,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K25" s="21" t="s">
         <v>20</v>
@@ -4922,7 +4915,7 @@
         <v>52</v>
       </c>
       <c r="O25" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P25" s="39" t="s">
         <v>19</v>
@@ -4931,16 +4924,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S25" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S25" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T25" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="U25" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4954,12 +4947,12 @@
         <v>123</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="14"/>
       <c r="G26" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
@@ -4968,7 +4961,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>20</v>
@@ -4981,7 +4974,7 @@
         <v>54</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P26" s="39" t="s">
         <v>19</v>
@@ -4990,16 +4983,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S26" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S26" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T26" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U26" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5013,12 +5006,12 @@
         <v>123</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="14"/>
       <c r="G27" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H27" s="34">
         <v>25</v>
@@ -5027,7 +5020,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>20</v>
@@ -5040,7 +5033,7 @@
         <v>54</v>
       </c>
       <c r="O27" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P27" s="39" t="s">
         <v>19</v>
@@ -5049,16 +5042,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S27" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S27" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T27" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U27" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5072,12 +5065,12 @@
         <v>123</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="14"/>
       <c r="G28" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H28" s="27">
         <v>26</v>
@@ -5086,7 +5079,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>20</v>
@@ -5099,7 +5092,7 @@
         <v>54</v>
       </c>
       <c r="O28" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P28" s="39" t="s">
         <v>19</v>
@@ -5108,16 +5101,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S28" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S28" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T28" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U28" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5131,7 +5124,7 @@
         <v>123</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="14"/>
@@ -5145,7 +5138,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>20</v>
@@ -5176,12 +5169,12 @@
         <v>123</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="14"/>
       <c r="G30" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H30" s="27">
         <v>28</v>
@@ -5190,7 +5183,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>20</v>
@@ -5210,16 +5203,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S30" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S30" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T30" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U30" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5233,12 +5226,12 @@
         <v>123</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="14"/>
       <c r="G31" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H31" s="27">
         <v>29</v>
@@ -5247,7 +5240,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K31" s="21" t="s">
         <v>20</v>
@@ -5267,16 +5260,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="S31" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="S31" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="T31" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="U31" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
@@ -5466,6 +5459,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5480,12 +5479,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I31 P3:P31">

</xml_diff>

<commit_message>
Correcciones a nombres de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion04/ESCALETA CN_09_04_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion04/ESCALETA CN_09_04_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos E\Aula Planeta\Edición\Magda Gaviria\CN_09_04_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado09\guion04\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="258">
   <si>
     <t>Asignatura</t>
   </si>
@@ -398,9 +398,6 @@
     <t>La clasificación biológica a través del tiempo</t>
   </si>
   <si>
-    <t>Modelos de clasificación biológica</t>
-  </si>
-  <si>
     <t>La primera ficha explia qué es la clasificación biológica y por qué es importante. Segunda ficha explica el modelo tradicional de clasificación, con procariotas y eucariotas, y 5 reinos incluyendo el mónera. La tercera ficha explica los 3 dominios, con un reino cada uno de los dos primeros y con 4 reinos el eucariota. Se debe explicar que Archaea es en latín y arquea en español, lo mismo para Eukarya y Fungi.</t>
   </si>
   <si>
@@ -410,15 +407,9 @@
     <t xml:space="preserve">El modelo moderno  de clasificación </t>
   </si>
   <si>
-    <t>Diferencias entre el modelo tradicional y el moderno para clasificar los seres vivos</t>
-  </si>
-  <si>
     <t>Escribir diferencias entre ambos modelos, de manera que se ubiquen en el contenedor "Modelo tradicional" o "Modelo moderno"</t>
   </si>
   <si>
-    <t>Científicos destacados en el desarrollo de la clasificación biológica</t>
-  </si>
-  <si>
     <t>Interactivo que presenta algunos científicos destacados y sus aportes al desarrollo de la clasificación biológica</t>
   </si>
   <si>
@@ -452,9 +443,6 @@
     <t>Las categorías taxonómicas superiores</t>
   </si>
   <si>
-    <t>Fundamentos de la taxonomía</t>
-  </si>
-  <si>
     <t xml:space="preserve">Se debe hacer un texto con los términos taxa, taxón, análogos, homólogos y binomial. Expandir si se quiere. </t>
   </si>
   <si>
@@ -500,21 +488,6 @@
     <t>Bacteria: el dominio de las bacterias</t>
   </si>
   <si>
-    <t>Actividad acerca del dominio Bacteria</t>
-  </si>
-  <si>
-    <t>¿Cuáles son las características del dominio Eukarya?</t>
-  </si>
-  <si>
-    <t>¿Cuáles son las características del dominio Archaea?</t>
-  </si>
-  <si>
-    <t>¿Cuáles son las características del dominio Bacteria?</t>
-  </si>
-  <si>
-    <t>Actividad acerca del dominio Eukarya</t>
-  </si>
-  <si>
     <t>Las diferencias entre los tres dominios</t>
   </si>
   <si>
@@ -551,21 +524,9 @@
     <t>Actividad para reforzar lo aprendido sobre los reinos eucariotas</t>
   </si>
   <si>
-    <t>Actividad para reforzar lo aprendido sobre el reino archeobacteria</t>
-  </si>
-  <si>
-    <t>Actividad para reforzar lo aprendido sobre el reino eubacteria</t>
-  </si>
-  <si>
     <t>¿Qué sabes sobre los reinos eucariotas?</t>
   </si>
   <si>
-    <t>¿Qué sabes sobre el reino archeobacteria?</t>
-  </si>
-  <si>
-    <t>¿Qué sabes sobre el reino eubacteria?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Las respuestas a las preguntas son de tipo falso y verdadero </t>
   </si>
   <si>
@@ -705,9 +666,6 @@
   </si>
   <si>
     <t>Actividad acerca de la jerarquía de los taxones</t>
-  </si>
-  <si>
-    <t>Actividad en la que se debe indicar a qué categorías taxonómicas pertenecen algunos organismos</t>
   </si>
   <si>
     <t>¿A qué taxones perteneces estos organismos?</t>
@@ -768,9 +726,6 @@
     <t>Los seis reinos de la naturaleza</t>
   </si>
   <si>
-    <t>Interactivo acerca de los reinos eubacteria, archeobacteria, plantae, animalia, fungi y protista</t>
-  </si>
-  <si>
     <t xml:space="preserve">En el primer menú hay tres imáganes, una para cada dominio. Al entrar en cada imagen se llega al menú de los reinos (por tanto, la dos primeras imágenes llevan cada una a una sola imagen, los reinos archeobacteria y eubacteria. Si acaso el editor de recursos no dejara que haya sólo una imagen, se puede hacer una para características generales y otra para ejemplos, pero es preferible que todo esté en una sola imagen). La tercera imagen lleva a los 4 reinos procariotas, y al entrar a cada uno se hace una descripción del reino y se dan ejemplos. En los reinos procariotas se debe aclarar que realmente los dominios de arqueas y bacterias aún no se conocen lo sufuciente como para definir reinos, y hablar de uno en cada grupo es algo provisional. Al hablar de protistas se debe aclarar también que en este grupo se incluyen diversos organismos que probablemente pertenecen a varios reinos distintos, que aún hace falta definir. También se debe explicar que el término protoctistas es sinónimo de protistas. </t>
   </si>
   <si>
@@ -799,13 +754,340 @@
   </si>
   <si>
     <t>Recurso F6-03</t>
+  </si>
+  <si>
+    <t>Los modelos de clasificación biológica</t>
+  </si>
+  <si>
+    <t>Las diferencias entre el modelo tradicional y el moderno para clasificar a los seres vivos</t>
+  </si>
+  <si>
+    <t>Los científicos destacados en el desarrollo de la clasificación biológica</t>
+  </si>
+  <si>
+    <t>Los fundamentos de la taxonomía</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">¿Cuáles son las características del dominio </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Archaea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">¿Cuáles son las características del dominio </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bacteria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Actividad acerca del dominio </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bacteria</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">¿Cuáles son las características del dominio </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eukarya</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Actividad acerca del dominio </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eukarya</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Interactivo acerca de los reinos </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>eubacteria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>archeobacteria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>plantae</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>animalia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fungi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>protista</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>¿Qué sabes sobre el reino</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> eubacteria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">¿Qué sabes sobre el reino </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>archeobacteria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Actividad para reforzar lo aprendido sobre el reino </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>eubacteria</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Actividad para reforzar lo aprendido sobre el reino </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>archeobacteria</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -839,6 +1121,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1108,25 +1398,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1151,6 +1429,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3420,8 +3710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3432,7 +3722,7 @@
     <col min="4" max="4" width="34.140625" customWidth="1"/>
     <col min="5" max="5" width="32.85546875" customWidth="1"/>
     <col min="6" max="6" width="32.85546875" style="15" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" customWidth="1"/>
+    <col min="7" max="7" width="50" customWidth="1"/>
     <col min="8" max="9" width="18.28515625" style="15" customWidth="1"/>
     <col min="10" max="10" width="30.28515625" customWidth="1"/>
     <col min="11" max="11" width="18.85546875" customWidth="1"/>
@@ -3449,94 +3739,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="44" t="s">
+      <c r="N1" s="52"/>
+      <c r="O1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="43" t="s">
+      <c r="P1" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="45" t="s">
+      <c r="Q1" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="S1" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="U1" s="55" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="52"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="48"/>
       <c r="M2" s="13" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="55"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -3549,14 +3839,14 @@
         <v>123</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="E3" s="38" t="s">
         <v>124</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="35" t="s">
-        <v>125</v>
+        <v>244</v>
       </c>
       <c r="H3" s="34">
         <v>1</v>
@@ -3565,7 +3855,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="41" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="K3" s="21" t="s">
         <v>20</v>
@@ -3578,7 +3868,7 @@
       </c>
       <c r="N3" s="22"/>
       <c r="O3" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P3" s="39" t="s">
         <v>19</v>
@@ -3587,16 +3877,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="S3" s="24" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="T3" s="26" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="U3" s="24" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3610,14 +3900,14 @@
         <v>123</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="27"/>
       <c r="G4" s="28" t="s">
-        <v>129</v>
+        <v>245</v>
       </c>
       <c r="H4" s="27">
         <v>2</v>
@@ -3626,7 +3916,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>20</v>
@@ -3639,7 +3929,7 @@
         <v>43</v>
       </c>
       <c r="O4" s="27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P4" s="39" t="s">
         <v>19</v>
@@ -3648,16 +3938,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="31" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S4" s="30" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T4" s="32" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="U4" s="30" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3671,14 +3961,14 @@
         <v>123</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="28" t="s">
-        <v>131</v>
+        <v>246</v>
       </c>
       <c r="H5" s="27">
         <v>3</v>
@@ -3687,7 +3977,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K5" s="21" t="s">
         <v>20</v>
@@ -3700,7 +3990,7 @@
       </c>
       <c r="N5" s="22"/>
       <c r="O5" s="33" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="P5" s="39" t="s">
         <v>19</v>
@@ -3709,16 +3999,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="31" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="S5" s="30" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="T5" s="32" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="U5" s="30" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3732,14 +4022,14 @@
         <v>123</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="28" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="H6" s="27">
         <v>4</v>
@@ -3748,7 +4038,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>20</v>
@@ -3761,7 +4051,7 @@
         <v>52</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="P6" s="39" t="s">
         <v>19</v>
@@ -3770,16 +4060,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="31" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S6" s="30" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T6" s="32" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="U6" s="30" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3793,14 +4083,14 @@
         <v>123</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H7" s="34">
         <v>5</v>
@@ -3809,7 +4099,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K7" s="21" t="s">
         <v>20</v>
@@ -3822,7 +4112,7 @@
       </c>
       <c r="N7" s="22"/>
       <c r="O7" s="27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P7" s="39" t="s">
         <v>19</v>
@@ -3831,16 +4121,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="31" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="S7" s="30" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="T7" s="26" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="U7" s="30" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3854,14 +4144,14 @@
         <v>123</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="28" t="s">
-        <v>143</v>
+        <v>247</v>
       </c>
       <c r="H8" s="27">
         <v>6</v>
@@ -3870,7 +4160,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>20</v>
@@ -3883,7 +4173,7 @@
         <v>28</v>
       </c>
       <c r="O8" s="27" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="P8" s="39" t="s">
         <v>19</v>
@@ -3892,16 +4182,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="31" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S8" s="30" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T8" s="32" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="U8" s="30" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3915,14 +4205,14 @@
         <v>123</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="28" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H9" s="27">
         <v>7</v>
@@ -3931,7 +4221,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>20</v>
@@ -3944,7 +4234,7 @@
       </c>
       <c r="N9" s="22"/>
       <c r="O9" s="27" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="P9" s="39" t="s">
         <v>19</v>
@@ -3953,16 +4243,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="31" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="S9" s="30" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="T9" s="32" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="U9" s="30" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3976,14 +4266,14 @@
         <v>123</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="28" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="H10" s="27">
         <v>8</v>
@@ -3992,7 +4282,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>20</v>
@@ -4005,7 +4295,7 @@
         <v>45</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="P10" s="39" t="s">
         <v>19</v>
@@ -4014,16 +4304,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="U10" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4037,16 +4327,16 @@
         <v>123</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H11" s="27">
         <v>9</v>
@@ -4055,7 +4345,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>19</v>
@@ -4066,25 +4356,25 @@
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
       <c r="O11" s="27" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="P11" s="39" t="s">
         <v>19</v>
       </c>
       <c r="Q11" s="30" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="R11" s="31" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="S11" s="30" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="T11" s="32" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="U11" s="30" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4098,16 +4388,16 @@
         <v>123</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="H12" s="27">
         <v>10</v>
@@ -4116,7 +4406,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="29" t="s">
-        <v>228</v>
+        <v>130</v>
       </c>
       <c r="K12" s="21" t="s">
         <v>20</v>
@@ -4129,7 +4419,7 @@
         <v>43</v>
       </c>
       <c r="O12" s="27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="P12" s="39" t="s">
         <v>19</v>
@@ -4138,16 +4428,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S12" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="U12" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4161,16 +4451,16 @@
         <v>123</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H13" s="27">
         <v>11</v>
@@ -4179,7 +4469,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="29" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>20</v>
@@ -4192,7 +4482,7 @@
         <v>51</v>
       </c>
       <c r="O13" s="27" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="P13" s="39" t="s">
         <v>20</v>
@@ -4201,16 +4491,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="U13" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4224,14 +4514,14 @@
         <v>123</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="28" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="H14" s="27">
         <v>12</v>
@@ -4240,7 +4530,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K14" s="21" t="s">
         <v>20</v>
@@ -4253,7 +4543,7 @@
         <v>52</v>
       </c>
       <c r="O14" s="42" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="P14" s="39" t="s">
         <v>19</v>
@@ -4262,16 +4552,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4285,12 +4575,12 @@
         <v>123</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="14"/>
       <c r="G15" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H15" s="27">
         <v>13</v>
@@ -4299,7 +4589,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>20</v>
@@ -4312,7 +4602,7 @@
       </c>
       <c r="N15" s="12"/>
       <c r="O15" s="14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="P15" s="39" t="s">
         <v>19</v>
@@ -4321,16 +4611,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4344,14 +4634,14 @@
         <v>123</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="3" t="s">
-        <v>162</v>
+        <v>249</v>
       </c>
       <c r="H16" s="27">
         <v>14</v>
@@ -4360,7 +4650,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>159</v>
+        <v>250</v>
       </c>
       <c r="K16" s="21" t="s">
         <v>20</v>
@@ -4373,7 +4663,7 @@
         <v>27</v>
       </c>
       <c r="O16" s="14" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="P16" s="39" t="s">
         <v>19</v>
@@ -4382,16 +4672,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="U16" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4405,14 +4695,14 @@
         <v>123</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="3" t="s">
-        <v>161</v>
+        <v>248</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
@@ -4421,7 +4711,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="K17" s="21" t="s">
         <v>20</v>
@@ -4434,7 +4724,7 @@
         <v>27</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="P17" s="39" t="s">
         <v>19</v>
@@ -4443,16 +4733,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T17" s="7" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="U17" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4466,14 +4756,14 @@
         <v>123</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="3" t="s">
-        <v>160</v>
+        <v>251</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
@@ -4482,7 +4772,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>163</v>
+        <v>252</v>
       </c>
       <c r="K18" s="21" t="s">
         <v>20</v>
@@ -4495,7 +4785,7 @@
         <v>27</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="P18" s="39" t="s">
         <v>19</v>
@@ -4504,16 +4794,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4527,14 +4817,14 @@
         <v>123</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H19" s="27">
         <v>17</v>
@@ -4543,7 +4833,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>20</v>
@@ -4556,7 +4846,7 @@
         <v>43</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="P19" s="39" t="s">
         <v>20</v>
@@ -4565,16 +4855,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="U19" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4588,14 +4878,14 @@
         <v>123</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="3" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="H20" s="27">
         <v>18</v>
@@ -4604,7 +4894,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>20</v>
@@ -4617,7 +4907,7 @@
         <v>52</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="P20" s="39" t="s">
         <v>19</v>
@@ -4626,16 +4916,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S20" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4649,12 +4939,12 @@
         <v>123</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="14"/>
       <c r="G21" s="3" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="H21" s="34">
         <v>19</v>
@@ -4663,7 +4953,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="K21" s="21" t="s">
         <v>20</v>
@@ -4676,7 +4966,7 @@
       </c>
       <c r="N21" s="12"/>
       <c r="O21" s="14" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="P21" s="39" t="s">
         <v>19</v>
@@ -4685,16 +4975,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="S21" s="6" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="U21" s="6" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4708,14 +4998,14 @@
         <v>123</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="3" t="s">
-        <v>180</v>
+        <v>254</v>
       </c>
       <c r="H22" s="27">
         <v>20</v>
@@ -4724,7 +5014,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>177</v>
+        <v>256</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>20</v>
@@ -4737,7 +5027,7 @@
         <v>32</v>
       </c>
       <c r="O22" s="14" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="P22" s="39" t="s">
         <v>19</v>
@@ -4746,16 +5036,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="T22" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="S22" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="T22" s="7" t="s">
-        <v>219</v>
-      </c>
       <c r="U22" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4769,14 +5059,14 @@
         <v>123</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="3" t="s">
-        <v>179</v>
+        <v>255</v>
       </c>
       <c r="H23" s="27">
         <v>21</v>
@@ -4785,7 +5075,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>176</v>
+        <v>257</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>20</v>
@@ -4798,7 +5088,7 @@
         <v>32</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="P23" s="39" t="s">
         <v>19</v>
@@ -4807,16 +5097,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S23" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="T23" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="T23" s="7" t="s">
-        <v>220</v>
-      </c>
       <c r="U23" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4830,14 +5120,14 @@
         <v>123</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="3" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="H24" s="27">
         <v>22</v>
@@ -4846,7 +5136,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>20</v>
@@ -4859,7 +5149,7 @@
         <v>23</v>
       </c>
       <c r="O24" s="14" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="P24" s="39" t="s">
         <v>19</v>
@@ -4868,16 +5158,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T24" s="7" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="U24" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4891,14 +5181,14 @@
         <v>123</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="3" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="H25" s="27">
         <v>23</v>
@@ -4907,7 +5197,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="K25" s="21" t="s">
         <v>20</v>
@@ -4920,7 +5210,7 @@
         <v>52</v>
       </c>
       <c r="O25" s="14" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="P25" s="39" t="s">
         <v>19</v>
@@ -4929,16 +5219,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S25" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T25" s="7" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="U25" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4952,12 +5242,12 @@
         <v>123</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="14"/>
       <c r="G26" s="3" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
@@ -4966,7 +5256,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>20</v>
@@ -4979,7 +5269,7 @@
         <v>54</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="P26" s="39" t="s">
         <v>19</v>
@@ -4988,16 +5278,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S26" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T26" s="7" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="U26" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5011,12 +5301,12 @@
         <v>123</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="14"/>
       <c r="G27" s="3" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="H27" s="34">
         <v>25</v>
@@ -5025,7 +5315,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>20</v>
@@ -5038,7 +5328,7 @@
         <v>54</v>
       </c>
       <c r="O27" s="14" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="P27" s="39" t="s">
         <v>19</v>
@@ -5047,16 +5337,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S27" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="U27" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5070,12 +5360,12 @@
         <v>123</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="14"/>
       <c r="G28" s="3" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="H28" s="27">
         <v>26</v>
@@ -5084,7 +5374,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>20</v>
@@ -5097,7 +5387,7 @@
         <v>54</v>
       </c>
       <c r="O28" s="14" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="P28" s="39" t="s">
         <v>19</v>
@@ -5106,16 +5396,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S28" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T28" s="7" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="U28" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5129,7 +5419,7 @@
         <v>123</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="14"/>
@@ -5143,7 +5433,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>20</v>
@@ -5174,12 +5464,12 @@
         <v>123</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="14"/>
       <c r="G30" s="3" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="H30" s="27">
         <v>28</v>
@@ -5188,7 +5478,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>20</v>
@@ -5208,16 +5498,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S30" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T30" s="7" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="U30" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5231,12 +5521,12 @@
         <v>123</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="14"/>
       <c r="G31" s="3" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="H31" s="27">
         <v>29</v>
@@ -5245,7 +5535,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="K31" s="21" t="s">
         <v>20</v>
@@ -5265,16 +5555,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S31" s="6" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="U31" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
@@ -5464,6 +5754,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5478,12 +5774,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I31 P3:P31">

</xml_diff>

<commit_message>
Corrección motores en escaleta
Se cambian motores por restricción en el uso de f4, f13 y f13b
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion04/ESCALETA CN_09_04_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion04/ESCALETA CN_09_04_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado09\guion04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos E\Aula Planeta\Edición\Magda Gaviria\CN_09_04_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -398,9 +398,6 @@
     <t>La clasificación biológica a través del tiempo</t>
   </si>
   <si>
-    <t>La primera ficha explia qué es la clasificación biológica y por qué es importante. Segunda ficha explica el modelo tradicional de clasificación, con procariotas y eucariotas, y 5 reinos incluyendo el mónera. La tercera ficha explica los 3 dominios, con un reino cada uno de los dos primeros y con 4 reinos el eucariota. Se debe explicar que Archaea es en latín y arquea en español, lo mismo para Eukarya y Fungi.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Los representantes de la clasificación biológica   </t>
   </si>
   <si>
@@ -465,9 +462,6 @@
   </si>
   <si>
     <t>Las palabras de la sopa de letras don dominio, reino, filo, división, clase, orden, familia, género y especie</t>
-  </si>
-  <si>
-    <t>Una ficha para Bacterias, una para Archaeas y otra para Eukarya. Deben ser claras las diferencias entre dominios (ver cuaderno de estudio)</t>
   </si>
   <si>
     <t>Los dominios de la naturaleza</t>
@@ -1081,6 +1075,12 @@
       </rPr>
       <t>archeobacteria</t>
     </r>
+  </si>
+  <si>
+    <t>Una imagen de menú para Bacterias, una para Archaeas y otra para Eukarya. Deben ser claras las diferencias entre dominios (ver cuaderno de estudio)</t>
+  </si>
+  <si>
+    <t>La primera ficha explica qué es la clasificación biológica y por qué es importante. Segunda ficha explica el modelo tradicional de clasificación, con procariotas y eucariotas, y 5 reinos incluyendo el mónera. La tercera ficha explica los 3 dominios, con un reino cada uno de los dos primeros y con 4 reinos el eucariota. Se debe explicar que Archaea es en latín y arquea en español, lo mismo para Eukarya y Fungi.</t>
   </si>
 </sst>
 </file>
@@ -1398,13 +1398,25 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1429,18 +1441,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3710,8 +3710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3739,94 +3739,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="45" t="s">
+      <c r="N1" s="56"/>
+      <c r="O1" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="54" t="s">
+      <c r="P1" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="55" t="s">
+      <c r="Q1" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="55" t="s">
+      <c r="S1" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="56" t="s">
+      <c r="T1" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="55" t="s">
+      <c r="U1" s="45" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="48"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="13" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="55"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="45"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -3839,14 +3839,14 @@
         <v>123</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E3" s="38" t="s">
         <v>124</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="35" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H3" s="34">
         <v>1</v>
@@ -3855,7 +3855,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K3" s="21" t="s">
         <v>20</v>
@@ -3868,7 +3868,7 @@
       </c>
       <c r="N3" s="22"/>
       <c r="O3" s="23" t="s">
-        <v>125</v>
+        <v>257</v>
       </c>
       <c r="P3" s="39" t="s">
         <v>19</v>
@@ -3877,16 +3877,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="S3" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="T3" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="S3" s="24" t="s">
+      <c r="U3" s="24" t="s">
         <v>186</v>
-      </c>
-      <c r="T3" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="U3" s="24" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3900,14 +3900,14 @@
         <v>123</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" s="27"/>
       <c r="G4" s="28" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H4" s="27">
         <v>2</v>
@@ -3916,7 +3916,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>20</v>
@@ -3929,7 +3929,7 @@
         <v>43</v>
       </c>
       <c r="O4" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P4" s="39" t="s">
         <v>19</v>
@@ -3938,16 +3938,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S4" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="T4" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="U4" s="30" t="s">
         <v>194</v>
-      </c>
-      <c r="T4" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="U4" s="30" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3961,14 +3961,14 @@
         <v>123</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="28" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H5" s="27">
         <v>3</v>
@@ -3977,7 +3977,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K5" s="21" t="s">
         <v>20</v>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="N5" s="22"/>
       <c r="O5" s="33" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="P5" s="39" t="s">
         <v>19</v>
@@ -3999,16 +3999,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="S5" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="T5" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="U5" s="30" t="s">
         <v>186</v>
-      </c>
-      <c r="T5" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="U5" s="30" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4022,14 +4022,14 @@
         <v>123</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H6" s="27">
         <v>4</v>
@@ -4038,7 +4038,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>20</v>
@@ -4051,7 +4051,7 @@
         <v>52</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P6" s="39" t="s">
         <v>19</v>
@@ -4060,16 +4060,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="S6" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="T6" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="S6" s="30" t="s">
+      <c r="U6" s="30" t="s">
         <v>194</v>
-      </c>
-      <c r="T6" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="U6" s="30" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4083,14 +4083,14 @@
         <v>123</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H7" s="34">
         <v>5</v>
@@ -4099,7 +4099,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K7" s="21" t="s">
         <v>20</v>
@@ -4112,7 +4112,7 @@
       </c>
       <c r="N7" s="22"/>
       <c r="O7" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P7" s="39" t="s">
         <v>19</v>
@@ -4121,16 +4121,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="S7" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="T7" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="U7" s="30" t="s">
         <v>186</v>
-      </c>
-      <c r="T7" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="U7" s="30" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4144,14 +4144,14 @@
         <v>123</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="28" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H8" s="27">
         <v>6</v>
@@ -4160,7 +4160,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>20</v>
@@ -4173,7 +4173,7 @@
         <v>28</v>
       </c>
       <c r="O8" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P8" s="39" t="s">
         <v>19</v>
@@ -4182,16 +4182,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S8" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="T8" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="U8" s="30" t="s">
         <v>194</v>
-      </c>
-      <c r="T8" s="32" t="s">
-        <v>202</v>
-      </c>
-      <c r="U8" s="30" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4205,14 +4205,14 @@
         <v>123</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H9" s="27">
         <v>7</v>
@@ -4221,7 +4221,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>20</v>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="N9" s="22"/>
       <c r="O9" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P9" s="39" t="s">
         <v>19</v>
@@ -4243,16 +4243,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="S9" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="T9" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="U9" s="30" t="s">
         <v>186</v>
-      </c>
-      <c r="T9" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="U9" s="30" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4266,14 +4266,14 @@
         <v>123</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H10" s="27">
         <v>8</v>
@@ -4282,7 +4282,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>20</v>
@@ -4295,7 +4295,7 @@
         <v>45</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="P10" s="39" t="s">
         <v>19</v>
@@ -4304,16 +4304,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S10" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="U10" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T10" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4327,16 +4327,16 @@
         <v>123</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="F11" s="27" t="s">
-        <v>139</v>
-      </c>
       <c r="G11" s="28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H11" s="27">
         <v>9</v>
@@ -4345,7 +4345,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>19</v>
@@ -4356,25 +4356,25 @@
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
       <c r="O11" s="27" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="P11" s="39" t="s">
         <v>19</v>
       </c>
       <c r="Q11" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="R11" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="S11" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="R11" s="31" t="s">
+      <c r="T11" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="S11" s="30" t="s">
+      <c r="U11" s="30" t="s">
         <v>182</v>
-      </c>
-      <c r="T11" s="32" t="s">
-        <v>183</v>
-      </c>
-      <c r="U11" s="30" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4388,16 +4388,16 @@
         <v>123</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>139</v>
-      </c>
       <c r="G12" s="28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H12" s="27">
         <v>10</v>
@@ -4406,7 +4406,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K12" s="21" t="s">
         <v>20</v>
@@ -4419,7 +4419,7 @@
         <v>43</v>
       </c>
       <c r="O12" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P12" s="39" t="s">
         <v>19</v>
@@ -4428,16 +4428,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S12" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="U12" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T12" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="U12" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4451,16 +4451,16 @@
         <v>123</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="F13" s="27" t="s">
-        <v>139</v>
-      </c>
       <c r="G13" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H13" s="27">
         <v>11</v>
@@ -4469,7 +4469,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>20</v>
@@ -4482,7 +4482,7 @@
         <v>51</v>
       </c>
       <c r="O13" s="27" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="P13" s="39" t="s">
         <v>20</v>
@@ -4491,16 +4491,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S13" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T13" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="U13" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T13" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="U13" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4514,14 +4514,14 @@
         <v>123</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H14" s="27">
         <v>12</v>
@@ -4530,7 +4530,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K14" s="21" t="s">
         <v>20</v>
@@ -4543,7 +4543,7 @@
         <v>52</v>
       </c>
       <c r="O14" s="42" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P14" s="39" t="s">
         <v>19</v>
@@ -4552,16 +4552,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S14" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="U14" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T14" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="U14" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4575,12 +4575,12 @@
         <v>123</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="14"/>
       <c r="G15" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H15" s="27">
         <v>13</v>
@@ -4589,7 +4589,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>20</v>
@@ -4602,7 +4602,7 @@
       </c>
       <c r="N15" s="12"/>
       <c r="O15" s="14" t="s">
-        <v>148</v>
+        <v>256</v>
       </c>
       <c r="P15" s="39" t="s">
         <v>19</v>
@@ -4611,16 +4611,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="S15" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="U15" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="T15" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="U15" s="6" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4634,14 +4634,14 @@
         <v>123</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H16" s="27">
         <v>14</v>
@@ -4650,7 +4650,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="K16" s="21" t="s">
         <v>20</v>
@@ -4663,7 +4663,7 @@
         <v>27</v>
       </c>
       <c r="O16" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P16" s="39" t="s">
         <v>19</v>
@@ -4672,16 +4672,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S16" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="U16" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T16" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="U16" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4695,14 +4695,14 @@
         <v>123</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
@@ -4711,7 +4711,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K17" s="21" t="s">
         <v>20</v>
@@ -4724,7 +4724,7 @@
         <v>27</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P17" s="39" t="s">
         <v>19</v>
@@ -4733,16 +4733,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S17" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="U17" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T17" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="U17" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4756,14 +4756,14 @@
         <v>123</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
@@ -4772,7 +4772,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K18" s="21" t="s">
         <v>20</v>
@@ -4785,7 +4785,7 @@
         <v>27</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P18" s="39" t="s">
         <v>19</v>
@@ -4794,16 +4794,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S18" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="U18" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T18" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="U18" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4817,14 +4817,14 @@
         <v>123</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H19" s="27">
         <v>17</v>
@@ -4833,7 +4833,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>20</v>
@@ -4846,7 +4846,7 @@
         <v>43</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P19" s="39" t="s">
         <v>20</v>
@@ -4855,16 +4855,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S19" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="U19" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T19" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="U19" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4878,14 +4878,14 @@
         <v>123</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H20" s="27">
         <v>18</v>
@@ -4894,7 +4894,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>20</v>
@@ -4907,7 +4907,7 @@
         <v>52</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P20" s="39" t="s">
         <v>19</v>
@@ -4916,16 +4916,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S20" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T20" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="U20" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T20" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="U20" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4939,12 +4939,12 @@
         <v>123</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="14"/>
       <c r="G21" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H21" s="34">
         <v>19</v>
@@ -4953,7 +4953,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K21" s="21" t="s">
         <v>20</v>
@@ -4966,7 +4966,7 @@
       </c>
       <c r="N21" s="12"/>
       <c r="O21" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="P21" s="39" t="s">
         <v>19</v>
@@ -4975,16 +4975,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="S21" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="T21" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="U21" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="T21" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="U21" s="6" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4998,14 +4998,14 @@
         <v>123</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H22" s="27">
         <v>20</v>
@@ -5014,7 +5014,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>20</v>
@@ -5027,7 +5027,7 @@
         <v>32</v>
       </c>
       <c r="O22" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P22" s="39" t="s">
         <v>19</v>
@@ -5036,16 +5036,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S22" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="U22" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T22" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5059,14 +5059,14 @@
         <v>123</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H23" s="27">
         <v>21</v>
@@ -5075,7 +5075,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>20</v>
@@ -5088,7 +5088,7 @@
         <v>32</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P23" s="39" t="s">
         <v>19</v>
@@ -5097,16 +5097,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S23" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="U23" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T23" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="U23" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5120,14 +5120,14 @@
         <v>123</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H24" s="27">
         <v>22</v>
@@ -5136,7 +5136,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>20</v>
@@ -5149,7 +5149,7 @@
         <v>23</v>
       </c>
       <c r="O24" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="P24" s="39" t="s">
         <v>19</v>
@@ -5158,16 +5158,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S24" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="U24" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T24" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="U24" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5181,14 +5181,14 @@
         <v>123</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H25" s="27">
         <v>23</v>
@@ -5197,7 +5197,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K25" s="21" t="s">
         <v>20</v>
@@ -5210,7 +5210,7 @@
         <v>52</v>
       </c>
       <c r="O25" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P25" s="39" t="s">
         <v>19</v>
@@ -5219,16 +5219,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S25" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="U25" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T25" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="U25" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5242,12 +5242,12 @@
         <v>123</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="14"/>
       <c r="G26" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
@@ -5256,7 +5256,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>20</v>
@@ -5269,7 +5269,7 @@
         <v>54</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="P26" s="39" t="s">
         <v>19</v>
@@ -5278,16 +5278,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S26" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="U26" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T26" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="U26" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5301,12 +5301,12 @@
         <v>123</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="14"/>
       <c r="G27" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H27" s="34">
         <v>25</v>
@@ -5315,7 +5315,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>20</v>
@@ -5328,7 +5328,7 @@
         <v>54</v>
       </c>
       <c r="O27" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="P27" s="39" t="s">
         <v>19</v>
@@ -5337,16 +5337,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S27" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T27" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="U27" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T27" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="U27" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5360,12 +5360,12 @@
         <v>123</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="14"/>
       <c r="G28" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H28" s="27">
         <v>26</v>
@@ -5374,7 +5374,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>20</v>
@@ -5387,7 +5387,7 @@
         <v>54</v>
       </c>
       <c r="O28" s="14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="P28" s="39" t="s">
         <v>19</v>
@@ -5396,16 +5396,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S28" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T28" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="U28" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T28" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="U28" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5419,7 +5419,7 @@
         <v>123</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="14"/>
@@ -5433,7 +5433,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>20</v>
@@ -5464,12 +5464,12 @@
         <v>123</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="14"/>
       <c r="G30" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H30" s="27">
         <v>28</v>
@@ -5478,7 +5478,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>20</v>
@@ -5498,16 +5498,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S30" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T30" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="U30" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T30" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="U30" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5521,12 +5521,12 @@
         <v>123</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="14"/>
       <c r="G31" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H31" s="27">
         <v>29</v>
@@ -5535,7 +5535,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K31" s="21" t="s">
         <v>20</v>
@@ -5555,16 +5555,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S31" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T31" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="U31" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="T31" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="U31" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
@@ -5754,12 +5754,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5774,6 +5768,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I31 P3:P31">

</xml_diff>